<commit_message>
Required tables are all finished! except the one about the preprocessing of X, test en cours.
</commit_message>
<xml_diff>
--- a/Others/TestCuts/18TestCut2SeuilFunc2+addmipstart/pre_cut2_seuil_func_2_mipstart.xlsx
+++ b/Others/TestCuts/18TestCut2SeuilFunc2+addmipstart/pre_cut2_seuil_func_2_mipstart.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="pre_cut2_seuil_func_2_mipstart" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="681">
   <si>
     <t>Sc(N/M)</t>
   </si>
@@ -2050,6 +2050,18 @@
   </si>
   <si>
     <t xml:space="preserve"> 1814.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 348407.82</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 233094.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.61</t>
   </si>
 </sst>
 </file>
@@ -2861,7 +2873,7 @@
   <dimension ref="A1:O138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,7 +2928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2963,7 +2975,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2974,43 +2986,43 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>677</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>492</v>
+        <v>516</v>
       </c>
       <c r="L3">
-        <v>492</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>678</v>
       </c>
       <c r="O3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3021,43 +3033,43 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>679</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>492</v>
+        <v>444</v>
       </c>
       <c r="L4">
-        <v>492</v>
+        <v>73</v>
       </c>
       <c r="M4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>17</v>
+        <v>680</v>
       </c>
       <c r="O4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3104,7 +3116,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3151,7 +3163,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3198,7 +3210,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3245,7 +3257,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -3292,7 +3304,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3339,7 +3351,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -3386,7 +3398,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -3433,7 +3445,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -3480,7 +3492,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -3527,7 +3539,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -3574,7 +3586,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3621,7 +3633,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -3668,7 +3680,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3715,7 +3727,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -3762,7 +3774,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -3809,7 +3821,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -3856,7 +3868,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -3903,7 +3915,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -3950,7 +3962,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -3997,7 +4009,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -4044,7 +4056,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -4091,7 +4103,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -4138,7 +4150,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -4185,7 +4197,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -4232,7 +4244,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -4279,7 +4291,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -4326,7 +4338,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -4373,7 +4385,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -4420,7 +4432,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>124</v>
       </c>
@@ -4467,7 +4479,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -4514,7 +4526,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>134</v>
       </c>
@@ -4561,7 +4573,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -4608,7 +4620,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -4655,7 +4667,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -4702,7 +4714,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4749,7 +4761,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>157</v>
       </c>
@@ -4796,7 +4808,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>162</v>
       </c>
@@ -4843,7 +4855,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -4890,7 +4902,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>171</v>
       </c>
@@ -4937,7 +4949,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>175</v>
       </c>
@@ -4984,7 +4996,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>179</v>
       </c>
@@ -5031,7 +5043,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>183</v>
       </c>
@@ -5078,7 +5090,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>189</v>
       </c>
@@ -5125,7 +5137,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>193</v>
       </c>

</xml_diff>